<commit_message>
Found an error in Admittance matrix creation. Now fixed, and values are saved in vector Y, which is currently in the process of being put into matrix form.
</commit_message>
<xml_diff>
--- a/Data/Line_Data.xlsx
+++ b/Data/Line_Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC8E789-36E6-431B-9E55-3ACA682594E3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D566F3B-9A9D-4694-88F9-C48A67981CD3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,10 +17,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,7 +336,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,7 +369,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>0.5403</v>
+        <v>5.4030000000000002E-2</v>
       </c>
       <c r="D2">
         <v>0.22303999999999999</v>
@@ -427,7 +423,7 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>0.56950000000000001</v>
+        <v>5.6950000000000001E-2</v>
       </c>
       <c r="D5">
         <v>0.17388000000000001</v>

</xml_diff>